<commit_message>
Update Temas utilizados en parcial 2 OS.xlsx
</commit_message>
<xml_diff>
--- a/Temas utilizados en parcial 2 OS.xlsx
+++ b/Temas utilizados en parcial 2 OS.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UVG\2022\Semestre 1 2022\Sistemas operativos\Parcial 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0B02FE-FF6D-4727-8054-43F16D4C8CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47C1B1E-8C4D-40B4-B75A-D19948DBF231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35244" yWindow="2220" windowWidth="21540" windowHeight="11472" xr2:uid="{2A9D1636-F084-499E-9409-AC6FC4599738}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2A9D1636-F084-499E-9409-AC6FC4599738}"/>
   </bookViews>
   <sheets>
     <sheet name="Listado de temas" sheetId="1" r:id="rId1"/>
+    <sheet name="PREMISA" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Listado de temas'!$B$1:$E$39</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="85">
   <si>
     <t>Race condition</t>
   </si>
@@ -88,9 +89,6 @@
     <t>segmentacion y tabla de segmentos</t>
   </si>
   <si>
-    <t>fragemntacion interna y externa</t>
-  </si>
-  <si>
     <t>linking dinamico y estatico</t>
   </si>
   <si>
@@ -275,6 +273,27 @@
   </si>
   <si>
     <t xml:space="preserve">Transifiere paginas de memoria principal a secundaria y viceversa ; </t>
+  </si>
+  <si>
+    <t>Contorladores/drivers permiten la comunicacion de perifiericos con el CPU</t>
+  </si>
+  <si>
+    <t>GEMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Gema de la mente</t>
+  </si>
+  <si>
+    <t>Gema del poder</t>
+  </si>
+  <si>
+    <t>JUSTIFICACION</t>
+  </si>
+  <si>
+    <t>En el cuento/alegoria el sistema operativo ThanOS esta buscando administrar los temas del infinito; Estos son los aspectos clave de un ordenador y al administrarlos conseguir balance . En la primera escena ya tiene control del filesystem (gema del poder) con la cual controla como se almacenan y recuperan los datos almacenados en memoria. Luego logra dominar al disco duro y obtiene el tema del almacenamiento en memoria secundaria.  Despues vemos como habla con un proceso y le explica como todo es mas ordenado ahora que el los administra.</t>
   </si>
 </sst>
 </file>
@@ -304,7 +323,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -327,11 +346,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -344,6 +372,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3AA053-65E8-461B-9C1B-C05AE7207357}">
-  <dimension ref="B1:E47"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,453 +709,714 @@
     <col min="3" max="3" width="42.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.33203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="39.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E14" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E15" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
+      <c r="D21" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B27" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B30" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="E30" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="E31" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C32" s="3" t="s">
-        <v>30</v>
+      <c r="E32" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>47</v>
+        <v>75</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C39" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D47" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:E39" xr:uid="{FA3AA053-65E8-461B-9C1B-C05AE7207357}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1CEFCF-97E2-4FB4-94B4-E8A1572A66D7}">
+  <dimension ref="C5:M18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C5" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C5:M18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>